<commit_message>
fix PYTHONPATH + path to data
</commit_message>
<xml_diff>
--- a/tests/test_data/01_raw/abuse-ornl/ornl-testfile.xlsx
+++ b/tests/test_data/01_raw/abuse-ornl/ornl-testfile.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hege/fork/battery-archive-sandbox/scripts/tests/test-data/abuse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hege/workspace/battery-archive-sandbox/tests/test_data/01_raw/abuse-ornl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E08E4DB-BBC1-064B-A7B7-7F00BB3D373D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BEE8F6-9E6C-2541-B567-DA2FC0C7DDBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25920" yWindow="1140" windowWidth="24640" windowHeight="25240" xr2:uid="{66C1F057-51BF-C84B-9F92-AC42F94C3932}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -430,12 +430,13 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>